<commit_message>
BackLog com simples alteração no layout
</commit_message>
<xml_diff>
--- a/documentacao/planilhas/BackLog.xlsx
+++ b/documentacao/planilhas/BackLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C25EE11-43C8-4BF4-8E57-A7A951F2E956}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5855272C-67B6-4D64-9601-ADF34E583DF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -209,7 +209,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -537,17 +537,6 @@
       <left style="double">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF000000"/>
-      </left>
       <right/>
       <top style="double">
         <color rgb="FF000000"/>
@@ -574,7 +563,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -653,7 +642,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -667,10 +655,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -956,7 +944,7 @@
   <dimension ref="B1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -967,13 +955,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4">
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="48" t="s">
         <v>2</v>
       </c>
     </row>
@@ -981,10 +969,10 @@
       <c r="B2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="46">
+      <c r="C2" s="45">
         <v>3</v>
       </c>
-      <c r="D2" s="47">
+      <c r="D2" s="46">
         <v>1</v>
       </c>
     </row>
@@ -1088,10 +1076,10 @@
       </c>
     </row>
     <row r="14" spans="2:4">
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="41" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="12" t="s">
@@ -1099,7 +1087,7 @@
       </c>
     </row>
     <row r="15" spans="2:4">
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="42" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="7">
@@ -1308,7 +1296,7 @@
       </c>
     </row>
     <row r="35" spans="2:4">
-      <c r="B35" s="44" t="s">
+      <c r="B35" s="43" t="s">
         <v>32</v>
       </c>
       <c r="C35" s="36" t="s">
@@ -1319,7 +1307,7 @@
       </c>
     </row>
     <row r="36" spans="2:4">
-      <c r="B36" s="40" t="s">
+      <c r="B36" s="37" t="s">
         <v>33</v>
       </c>
       <c r="C36" s="38">

</xml_diff>